<commit_message>
just to be safe
</commit_message>
<xml_diff>
--- a/Libft.xlsx
+++ b/Libft.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="41">
   <si>
     <t xml:space="preserve">Function</t>
   </si>
@@ -40,10 +40,10 @@
     <t xml:space="preserve">ft_atoi.c</t>
   </si>
   <si>
+    <t xml:space="preserve">x</t>
+  </si>
+  <si>
     <t xml:space="preserve">ft_bzero.c</t>
-  </si>
-  <si>
-    <t xml:space="preserve">x</t>
   </si>
   <si>
     <t xml:space="preserve">ft_calloc.c</t>
@@ -211,14 +211,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC55757"/>
-        <bgColor rgb="FF993366"/>
+        <fgColor rgb="FF45D776"/>
+        <bgColor rgb="FF339966"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF45D776"/>
-        <bgColor rgb="FF339966"/>
+        <fgColor rgb="FFC55757"/>
+        <bgColor rgb="FF993366"/>
       </patternFill>
     </fill>
   </fills>
@@ -401,7 +401,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -409,6 +409,18 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="10" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="11" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="5" borderId="10" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -417,47 +429,35 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="12" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="10" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="11" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="12" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="5" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="5" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="5" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="14" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="15" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="14" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="15" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -540,8 +540,8 @@
   </sheetPr>
   <dimension ref="B1:H36"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G14" activeCellId="0" sqref="G14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I4" activeCellId="0" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -575,21 +575,23 @@
       <c r="C3" s="6"/>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
-      <c r="F3" s="8"/>
+      <c r="F3" s="8" t="s">
+        <v>6</v>
+      </c>
       <c r="H3" s="0" t="n">
         <f aca="false">COUNTBLANK(F3:F36)</f>
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="9" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C4" s="10"/>
       <c r="D4" s="11"/>
       <c r="E4" s="11"/>
       <c r="F4" s="12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -609,7 +611,7 @@
       <c r="D6" s="11"/>
       <c r="E6" s="11"/>
       <c r="F6" s="12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -620,7 +622,7 @@
       <c r="D7" s="11"/>
       <c r="E7" s="11"/>
       <c r="F7" s="12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -631,7 +633,7 @@
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
       <c r="F8" s="12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -642,7 +644,7 @@
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
       <c r="F9" s="12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -653,7 +655,7 @@
       <c r="D10" s="11"/>
       <c r="E10" s="11"/>
       <c r="F10" s="12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -676,17 +678,19 @@
       <c r="D12" s="11"/>
       <c r="E12" s="11"/>
       <c r="F12" s="12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="13"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="15"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="12" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="9" t="s">
@@ -695,7 +699,9 @@
       <c r="C14" s="10"/>
       <c r="D14" s="11"/>
       <c r="E14" s="11"/>
-      <c r="F14" s="12"/>
+      <c r="F14" s="12" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="9" t="s">
@@ -705,7 +711,7 @@
       <c r="D15" s="11"/>
       <c r="E15" s="11"/>
       <c r="F15" s="12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -716,7 +722,7 @@
       <c r="D16" s="11"/>
       <c r="E16" s="11"/>
       <c r="F16" s="12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -772,7 +778,7 @@
       <c r="D22" s="11"/>
       <c r="E22" s="11"/>
       <c r="F22" s="12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -783,7 +789,7 @@
       <c r="D23" s="11"/>
       <c r="E23" s="11"/>
       <c r="F23" s="12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -812,7 +818,7 @@
       <c r="D26" s="17"/>
       <c r="E26" s="17"/>
       <c r="F26" s="18" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -823,7 +829,7 @@
       <c r="D27" s="11"/>
       <c r="E27" s="11"/>
       <c r="F27" s="12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -834,7 +840,7 @@
       <c r="D28" s="11"/>
       <c r="E28" s="11"/>
       <c r="F28" s="12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -854,17 +860,19 @@
       <c r="D30" s="11"/>
       <c r="E30" s="11"/>
       <c r="F30" s="12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="C31" s="13"/>
-      <c r="D31" s="14"/>
-      <c r="E31" s="14"/>
-      <c r="F31" s="15"/>
+      <c r="C31" s="10"/>
+      <c r="D31" s="11"/>
+      <c r="E31" s="11"/>
+      <c r="F31" s="12" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="9" t="s">
@@ -874,7 +882,7 @@
       <c r="D32" s="11"/>
       <c r="E32" s="11"/>
       <c r="F32" s="12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -903,7 +911,7 @@
       <c r="D35" s="11"/>
       <c r="E35" s="11"/>
       <c r="F35" s="12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -914,7 +922,7 @@
       <c r="D36" s="21"/>
       <c r="E36" s="21"/>
       <c r="F36" s="22" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>